<commit_message>
java2 Holder on Aug 03
</commit_message>
<xml_diff>
--- a/Selenium/input_data/Input.xlsx
+++ b/Selenium/input_data/Input.xlsx
@@ -4,12 +4,26 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="8580"/>
+    <workbookView windowWidth="22188" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -103,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1041,7 +1055,7 @@
   <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
@@ -1149,4 +1163,20 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mar 2025 selenium basic and basic java
</commit_message>
<xml_diff>
--- a/Selenium/input_data/Input.xlsx
+++ b/Selenium/input_data/Input.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -112,6 +113,12 @@
   </si>
   <si>
     <t>lpa6</t>
+  </si>
+  <si>
+    <t>RAvi teja</t>
+  </si>
+  <si>
+    <t>fisrnam</t>
   </si>
 </sst>
 </file>
@@ -1055,8 +1062,8 @@
   <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -1168,14 +1175,65 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>